<commit_message>
Added TestCase for Data driven Testing in Selenium
</commit_message>
<xml_diff>
--- a/MSelPractice/TestData/RegisterCust.xlsx
+++ b/MSelPractice/TestData/RegisterCust.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="108" windowWidth="16212" windowHeight="5808"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12180" windowHeight="4590"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -138,8 +139,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +225,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -302,6 +308,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -336,6 +343,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -511,25 +519,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,7 +572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -599,7 +607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
@@ -634,7 +642,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -681,24 +689,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>